<commit_message>
added deployment date for plates
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pieter/Dropbox (IPOfI)/werk/projects/PacMAN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pieter/Desktop/pacman-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BCEA9C-9943-ED42-B8BD-47C8C3F611B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF16444-D71B-F840-8F20-BBD0A0E9D5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="27120" xr2:uid="{35AAA470-4882-944F-841D-C404D1D5A17A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="126">
   <si>
     <t>Port name</t>
   </si>
@@ -341,9 +341,6 @@
     <t>SRA data</t>
   </si>
   <si>
-    <t>0.1.0</t>
-  </si>
-  <si>
     <t>Target gene</t>
   </si>
   <si>
@@ -414,6 +411,12 @@
   </si>
   <si>
     <t>p.provoost@unesco.org</t>
+  </si>
+  <si>
+    <t>Deployment date</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1080,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1160,7 +1163,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="58" t="s">
         <v>29</v>
@@ -1168,10 +1171,10 @@
     </row>
     <row r="9" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="59" t="s">
         <v>123</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1188,7 +1191,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2282,10 +2285,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{592FA8E1-B0CB-844C-B673-47D7A564EE3C}">
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2293,26 +2296,26 @@
     <col min="1" max="1" width="4.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="5" width="10.83203125" style="3"/>
-    <col min="6" max="7" width="10.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="3"/>
-    <col min="9" max="9" width="17.6640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="3"/>
-    <col min="11" max="11" width="15.6640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="14.1640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="3"/>
-    <col min="14" max="14" width="12.6640625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="13.83203125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="22.6640625" style="3" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="3"/>
+    <col min="6" max="8" width="10.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="3"/>
+    <col min="10" max="10" width="17.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="3"/>
+    <col min="12" max="12" width="15.6640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="3"/>
+    <col min="15" max="15" width="12.6640625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="22.6640625" style="3" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="7" t="s">
         <v>53</v>
       </c>
@@ -2332,34 +2335,37 @@
         <v>5</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D3" s="3" t="s">
         <v>38</v>
       </c>
@@ -2373,20 +2379,23 @@
         <v>34</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="L3" s="4" t="s">
+      <c r="J3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="M3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B4" s="15" t="s">
         <v>72</v>
       </c>
@@ -2395,25 +2404,26 @@
       <c r="E4" s="52"/>
       <c r="F4" s="53"/>
       <c r="G4" s="28"/>
-      <c r="H4" s="30">
+      <c r="H4" s="53"/>
+      <c r="I4" s="30">
         <v>0</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="30"/>
+      <c r="K4" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="54" t="s">
+      <c r="L4" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="30">
+      <c r="M4" s="30">
         <v>1</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="16"/>
+      <c r="N4" s="30"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="17"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P4" s="16"/>
+      <c r="Q4" s="17"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
         <v>73</v>
       </c>
@@ -2422,25 +2432,26 @@
       <c r="E5" s="44"/>
       <c r="F5" s="45"/>
       <c r="G5" s="35"/>
-      <c r="H5" s="37">
+      <c r="H5" s="45"/>
+      <c r="I5" s="37">
         <v>0</v>
       </c>
-      <c r="I5" s="37"/>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="37"/>
+      <c r="K5" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="K5" s="55" t="s">
+      <c r="L5" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="L5" s="37">
+      <c r="M5" s="37">
         <v>1</v>
       </c>
-      <c r="M5" s="37"/>
-      <c r="N5" s="19"/>
+      <c r="N5" s="37"/>
       <c r="O5" s="19"/>
-      <c r="P5" s="20"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P5" s="19"/>
+      <c r="Q5" s="20"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" s="18" t="s">
         <v>74</v>
       </c>
@@ -2449,25 +2460,26 @@
       <c r="E6" s="44"/>
       <c r="F6" s="45"/>
       <c r="G6" s="35"/>
-      <c r="H6" s="37">
+      <c r="H6" s="45"/>
+      <c r="I6" s="37">
         <v>0</v>
       </c>
-      <c r="I6" s="37"/>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="37"/>
+      <c r="K6" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="55" t="s">
+      <c r="L6" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="L6" s="37">
+      <c r="M6" s="37">
         <v>1</v>
       </c>
-      <c r="M6" s="37"/>
-      <c r="N6" s="19"/>
+      <c r="N6" s="37"/>
       <c r="O6" s="19"/>
-      <c r="P6" s="20"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P6" s="19"/>
+      <c r="Q6" s="20"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B7" s="18" t="s">
         <v>87</v>
       </c>
@@ -2478,23 +2490,24 @@
       <c r="E7" s="44"/>
       <c r="F7" s="45"/>
       <c r="G7" s="35"/>
-      <c r="H7" s="37">
+      <c r="H7" s="45"/>
+      <c r="I7" s="37">
         <v>10</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="37"/>
+      <c r="K7" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="K7" s="55"/>
-      <c r="L7" s="37"/>
+      <c r="L7" s="55"/>
       <c r="M7" s="37"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19" t="s">
+      <c r="N7" s="37"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="P7" s="20"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7" s="20"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B8" s="18" t="s">
         <v>88</v>
       </c>
@@ -2505,23 +2518,24 @@
       <c r="E8" s="44"/>
       <c r="F8" s="45"/>
       <c r="G8" s="35"/>
-      <c r="H8" s="37">
+      <c r="H8" s="45"/>
+      <c r="I8" s="37">
         <v>10</v>
       </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="37"/>
+      <c r="K8" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="K8" s="55"/>
-      <c r="L8" s="37"/>
+      <c r="L8" s="55"/>
       <c r="M8" s="37"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19" t="s">
+      <c r="N8" s="37"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="P8" s="20"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q8" s="20"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9" s="18" t="s">
         <v>89</v>
       </c>
@@ -2532,23 +2546,24 @@
       <c r="E9" s="44"/>
       <c r="F9" s="45"/>
       <c r="G9" s="35"/>
-      <c r="H9" s="37">
+      <c r="H9" s="45"/>
+      <c r="I9" s="37">
         <v>10</v>
       </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="37"/>
+      <c r="K9" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="K9" s="55"/>
-      <c r="L9" s="37"/>
+      <c r="L9" s="55"/>
       <c r="M9" s="37"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19" t="s">
+      <c r="N9" s="37"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="P9" s="20"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q9" s="20"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10" s="18" t="s">
         <v>90</v>
       </c>
@@ -2559,23 +2574,24 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="37">
+      <c r="H10" s="45"/>
+      <c r="I10" s="37">
         <v>10</v>
       </c>
-      <c r="I10" s="37"/>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="37"/>
+      <c r="K10" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="K10" s="55"/>
-      <c r="L10" s="19"/>
+      <c r="L10" s="55"/>
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
-      <c r="O10" s="19" t="s">
+      <c r="O10" s="19"/>
+      <c r="P10" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="P10" s="20"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q10" s="20"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B11" s="18" t="s">
         <v>91</v>
       </c>
@@ -2586,23 +2602,24 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="37">
+      <c r="H11" s="45"/>
+      <c r="I11" s="37">
         <v>10</v>
       </c>
-      <c r="I11" s="37"/>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="37"/>
+      <c r="K11" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="K11" s="55"/>
-      <c r="L11" s="19"/>
+      <c r="L11" s="55"/>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
-      <c r="O11" s="19" t="s">
+      <c r="O11" s="19"/>
+      <c r="P11" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="P11" s="20"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q11" s="20"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B12" s="18" t="s">
         <v>92</v>
       </c>
@@ -2613,23 +2630,24 @@
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="37">
+      <c r="H12" s="45"/>
+      <c r="I12" s="37">
         <v>10</v>
       </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="37"/>
+      <c r="K12" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="K12" s="55"/>
-      <c r="L12" s="19"/>
+      <c r="L12" s="55"/>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
-      <c r="O12" s="19" t="s">
+      <c r="O12" s="19"/>
+      <c r="P12" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="P12" s="20"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q12" s="20"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>83</v>
       </c>
@@ -2638,29 +2656,30 @@
       <c r="E13" s="44"/>
       <c r="F13" s="45"/>
       <c r="G13" s="35"/>
-      <c r="H13" s="37">
+      <c r="H13" s="45"/>
+      <c r="I13" s="37">
         <v>9</v>
       </c>
-      <c r="I13" s="37">
+      <c r="J13" s="37">
         <v>0</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="K13" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="55" t="s">
+      <c r="L13" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="37">
+      <c r="M13" s="37">
         <v>900</v>
       </c>
-      <c r="M13" s="37">
+      <c r="N13" s="37">
         <v>60</v>
       </c>
-      <c r="N13" s="19"/>
       <c r="O13" s="19"/>
-      <c r="P13" s="20"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P13" s="19"/>
+      <c r="Q13" s="20"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>84</v>
       </c>
@@ -2669,29 +2688,30 @@
       <c r="E14" s="44"/>
       <c r="F14" s="45"/>
       <c r="G14" s="35"/>
-      <c r="H14" s="37">
+      <c r="H14" s="45"/>
+      <c r="I14" s="37">
         <v>9</v>
       </c>
-      <c r="I14" s="37">
+      <c r="J14" s="37">
         <v>0</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="K14" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="55" t="s">
+      <c r="L14" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="L14" s="37">
+      <c r="M14" s="37">
         <v>900</v>
       </c>
-      <c r="M14" s="37">
+      <c r="N14" s="37">
         <v>60</v>
       </c>
-      <c r="N14" s="19"/>
       <c r="O14" s="19"/>
-      <c r="P14" s="20"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P14" s="19"/>
+      <c r="Q14" s="20"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
         <v>85</v>
       </c>
@@ -2700,29 +2720,30 @@
       <c r="E15" s="44"/>
       <c r="F15" s="45"/>
       <c r="G15" s="35"/>
-      <c r="H15" s="37">
+      <c r="H15" s="45"/>
+      <c r="I15" s="37">
         <v>9</v>
       </c>
-      <c r="I15" s="37">
+      <c r="J15" s="37">
         <v>0</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="K15" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="K15" s="55" t="s">
+      <c r="L15" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="L15" s="37">
+      <c r="M15" s="37">
         <v>900</v>
       </c>
-      <c r="M15" s="37">
+      <c r="N15" s="37">
         <v>60</v>
       </c>
-      <c r="N15" s="19"/>
       <c r="O15" s="19"/>
-      <c r="P15" s="20"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P15" s="19"/>
+      <c r="Q15" s="20"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="18" t="s">
         <v>94</v>
       </c>
@@ -2731,21 +2752,22 @@
       <c r="E16" s="44"/>
       <c r="F16" s="45"/>
       <c r="G16" s="35"/>
-      <c r="H16" s="37"/>
+      <c r="H16" s="45"/>
       <c r="I16" s="37"/>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="37"/>
+      <c r="K16" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="55" t="s">
+      <c r="L16" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="L16" s="37"/>
       <c r="M16" s="37"/>
-      <c r="N16" s="19"/>
+      <c r="N16" s="37"/>
       <c r="O16" s="19"/>
-      <c r="P16" s="20"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P16" s="19"/>
+      <c r="Q16" s="20"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
         <v>95</v>
       </c>
@@ -2754,21 +2776,22 @@
       <c r="E17" s="44"/>
       <c r="F17" s="45"/>
       <c r="G17" s="35"/>
-      <c r="H17" s="37"/>
+      <c r="H17" s="45"/>
       <c r="I17" s="37"/>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="37"/>
+      <c r="K17" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="K17" s="55" t="s">
+      <c r="L17" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="L17" s="37"/>
       <c r="M17" s="37"/>
-      <c r="N17" s="19"/>
+      <c r="N17" s="37"/>
       <c r="O17" s="19"/>
-      <c r="P17" s="20"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P17" s="19"/>
+      <c r="Q17" s="20"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" s="18" t="s">
         <v>96</v>
       </c>
@@ -2777,485 +2800,512 @@
       <c r="E18" s="44"/>
       <c r="F18" s="45"/>
       <c r="G18" s="35"/>
-      <c r="H18" s="37"/>
+      <c r="H18" s="45"/>
       <c r="I18" s="37"/>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="37"/>
+      <c r="K18" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="K18" s="55" t="s">
+      <c r="L18" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="L18" s="37"/>
       <c r="M18" s="37"/>
-      <c r="N18" s="19"/>
+      <c r="N18" s="37"/>
       <c r="O18" s="19"/>
-      <c r="P18" s="20"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P18" s="19"/>
+      <c r="Q18" s="20"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
       <c r="D19" s="44"/>
       <c r="E19" s="44"/>
       <c r="F19" s="45"/>
       <c r="G19" s="35"/>
-      <c r="H19" s="37"/>
+      <c r="H19" s="45"/>
       <c r="I19" s="37"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="55"/>
-      <c r="L19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="55"/>
       <c r="M19" s="37"/>
-      <c r="N19" s="19"/>
+      <c r="N19" s="37"/>
       <c r="O19" s="19"/>
-      <c r="P19" s="20"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P19" s="19"/>
+      <c r="Q19" s="20"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
       <c r="D20" s="44"/>
       <c r="E20" s="44"/>
       <c r="F20" s="45"/>
       <c r="G20" s="35"/>
-      <c r="H20" s="37"/>
+      <c r="H20" s="45"/>
       <c r="I20" s="37"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="55"/>
       <c r="M20" s="37"/>
-      <c r="N20" s="19"/>
+      <c r="N20" s="37"/>
       <c r="O20" s="19"/>
-      <c r="P20" s="20"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P20" s="19"/>
+      <c r="Q20" s="20"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
       <c r="D21" s="44"/>
       <c r="E21" s="44"/>
       <c r="F21" s="45"/>
       <c r="G21" s="35"/>
-      <c r="H21" s="37"/>
+      <c r="H21" s="45"/>
       <c r="I21" s="37"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="55"/>
       <c r="M21" s="37"/>
-      <c r="N21" s="19"/>
+      <c r="N21" s="37"/>
       <c r="O21" s="19"/>
-      <c r="P21" s="20"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P21" s="19"/>
+      <c r="Q21" s="20"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
       <c r="D22" s="44"/>
       <c r="E22" s="44"/>
       <c r="F22" s="45"/>
       <c r="G22" s="35"/>
-      <c r="H22" s="37"/>
+      <c r="H22" s="45"/>
       <c r="I22" s="37"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="55"/>
       <c r="M22" s="37"/>
-      <c r="N22" s="19"/>
+      <c r="N22" s="37"/>
       <c r="O22" s="19"/>
-      <c r="P22" s="20"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P22" s="19"/>
+      <c r="Q22" s="20"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23" s="18"/>
       <c r="C23" s="19"/>
       <c r="D23" s="44"/>
       <c r="E23" s="44"/>
       <c r="F23" s="45"/>
       <c r="G23" s="35"/>
-      <c r="H23" s="37"/>
+      <c r="H23" s="45"/>
       <c r="I23" s="37"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="55"/>
       <c r="M23" s="37"/>
-      <c r="N23" s="19"/>
+      <c r="N23" s="37"/>
       <c r="O23" s="19"/>
-      <c r="P23" s="20"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P23" s="19"/>
+      <c r="Q23" s="20"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
       <c r="D24" s="44"/>
       <c r="E24" s="44"/>
       <c r="F24" s="45"/>
       <c r="G24" s="35"/>
-      <c r="H24" s="37"/>
+      <c r="H24" s="45"/>
       <c r="I24" s="37"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="55"/>
-      <c r="L24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="55"/>
       <c r="M24" s="37"/>
-      <c r="N24" s="19"/>
+      <c r="N24" s="37"/>
       <c r="O24" s="19"/>
-      <c r="P24" s="20"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P24" s="19"/>
+      <c r="Q24" s="20"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" s="18"/>
       <c r="C25" s="19"/>
       <c r="D25" s="44"/>
       <c r="E25" s="44"/>
       <c r="F25" s="45"/>
       <c r="G25" s="35"/>
-      <c r="H25" s="37"/>
+      <c r="H25" s="45"/>
       <c r="I25" s="37"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="55"/>
       <c r="M25" s="37"/>
-      <c r="N25" s="19"/>
+      <c r="N25" s="37"/>
       <c r="O25" s="19"/>
-      <c r="P25" s="20"/>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P25" s="19"/>
+      <c r="Q25" s="20"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
       <c r="D26" s="44"/>
       <c r="E26" s="44"/>
       <c r="F26" s="45"/>
       <c r="G26" s="35"/>
-      <c r="H26" s="37"/>
+      <c r="H26" s="45"/>
       <c r="I26" s="37"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="55"/>
       <c r="M26" s="37"/>
-      <c r="N26" s="19"/>
+      <c r="N26" s="37"/>
       <c r="O26" s="19"/>
-      <c r="P26" s="20"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P26" s="19"/>
+      <c r="Q26" s="20"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" s="18"/>
       <c r="C27" s="19"/>
       <c r="D27" s="44"/>
       <c r="E27" s="44"/>
       <c r="F27" s="45"/>
       <c r="G27" s="35"/>
-      <c r="H27" s="37"/>
+      <c r="H27" s="45"/>
       <c r="I27" s="37"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="55"/>
-      <c r="L27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="55"/>
       <c r="M27" s="37"/>
-      <c r="N27" s="19"/>
+      <c r="N27" s="37"/>
       <c r="O27" s="19"/>
-      <c r="P27" s="20"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P27" s="19"/>
+      <c r="Q27" s="20"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
       <c r="D28" s="44"/>
       <c r="E28" s="44"/>
       <c r="F28" s="45"/>
       <c r="G28" s="35"/>
-      <c r="H28" s="37"/>
+      <c r="H28" s="45"/>
       <c r="I28" s="37"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="55"/>
       <c r="M28" s="37"/>
-      <c r="N28" s="19"/>
+      <c r="N28" s="37"/>
       <c r="O28" s="19"/>
-      <c r="P28" s="20"/>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P28" s="19"/>
+      <c r="Q28" s="20"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
       <c r="D29" s="44"/>
       <c r="E29" s="44"/>
       <c r="F29" s="45"/>
       <c r="G29" s="35"/>
-      <c r="H29" s="37"/>
+      <c r="H29" s="45"/>
       <c r="I29" s="37"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="55"/>
-      <c r="L29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="55"/>
       <c r="M29" s="37"/>
-      <c r="N29" s="19"/>
+      <c r="N29" s="37"/>
       <c r="O29" s="19"/>
-      <c r="P29" s="20"/>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P29" s="19"/>
+      <c r="Q29" s="20"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
       <c r="D30" s="44"/>
       <c r="E30" s="44"/>
       <c r="F30" s="45"/>
       <c r="G30" s="35"/>
-      <c r="H30" s="37"/>
+      <c r="H30" s="45"/>
       <c r="I30" s="37"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="55"/>
       <c r="M30" s="37"/>
-      <c r="N30" s="19"/>
+      <c r="N30" s="37"/>
       <c r="O30" s="19"/>
-      <c r="P30" s="20"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P30" s="19"/>
+      <c r="Q30" s="20"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B31" s="18"/>
       <c r="C31" s="19"/>
       <c r="D31" s="44"/>
       <c r="E31" s="44"/>
       <c r="F31" s="45"/>
       <c r="G31" s="35"/>
-      <c r="H31" s="37"/>
+      <c r="H31" s="45"/>
       <c r="I31" s="37"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="55"/>
       <c r="M31" s="37"/>
-      <c r="N31" s="19"/>
+      <c r="N31" s="37"/>
       <c r="O31" s="19"/>
-      <c r="P31" s="20"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P31" s="19"/>
+      <c r="Q31" s="20"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B32" s="18"/>
       <c r="C32" s="19"/>
       <c r="D32" s="44"/>
       <c r="E32" s="44"/>
       <c r="F32" s="45"/>
       <c r="G32" s="35"/>
-      <c r="H32" s="37"/>
+      <c r="H32" s="45"/>
       <c r="I32" s="37"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="55"/>
       <c r="M32" s="37"/>
-      <c r="N32" s="19"/>
+      <c r="N32" s="37"/>
       <c r="O32" s="19"/>
-      <c r="P32" s="20"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P32" s="19"/>
+      <c r="Q32" s="20"/>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
       <c r="D33" s="44"/>
       <c r="E33" s="44"/>
       <c r="F33" s="45"/>
       <c r="G33" s="35"/>
-      <c r="H33" s="37"/>
+      <c r="H33" s="45"/>
       <c r="I33" s="37"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="37"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="55"/>
       <c r="M33" s="37"/>
-      <c r="N33" s="19"/>
+      <c r="N33" s="37"/>
       <c r="O33" s="19"/>
-      <c r="P33" s="20"/>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P33" s="19"/>
+      <c r="Q33" s="20"/>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
       <c r="D34" s="44"/>
       <c r="E34" s="44"/>
       <c r="F34" s="45"/>
       <c r="G34" s="35"/>
-      <c r="H34" s="37"/>
+      <c r="H34" s="45"/>
       <c r="I34" s="37"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="55"/>
-      <c r="L34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="55"/>
       <c r="M34" s="37"/>
-      <c r="N34" s="19"/>
+      <c r="N34" s="37"/>
       <c r="O34" s="19"/>
-      <c r="P34" s="20"/>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P34" s="19"/>
+      <c r="Q34" s="20"/>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" s="18"/>
       <c r="C35" s="19"/>
       <c r="D35" s="44"/>
       <c r="E35" s="44"/>
       <c r="F35" s="45"/>
       <c r="G35" s="35"/>
-      <c r="H35" s="37"/>
+      <c r="H35" s="45"/>
       <c r="I35" s="37"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="55"/>
-      <c r="L35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="55"/>
       <c r="M35" s="37"/>
-      <c r="N35" s="19"/>
+      <c r="N35" s="37"/>
       <c r="O35" s="19"/>
-      <c r="P35" s="20"/>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P35" s="19"/>
+      <c r="Q35" s="20"/>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B36" s="18"/>
       <c r="C36" s="19"/>
       <c r="D36" s="44"/>
       <c r="E36" s="44"/>
       <c r="F36" s="45"/>
       <c r="G36" s="35"/>
-      <c r="H36" s="37"/>
+      <c r="H36" s="45"/>
       <c r="I36" s="37"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="55"/>
-      <c r="L36" s="37"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="55"/>
       <c r="M36" s="37"/>
-      <c r="N36" s="19"/>
+      <c r="N36" s="37"/>
       <c r="O36" s="19"/>
-      <c r="P36" s="20"/>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P36" s="19"/>
+      <c r="Q36" s="20"/>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B37" s="18"/>
       <c r="C37" s="19"/>
       <c r="D37" s="44"/>
       <c r="E37" s="44"/>
       <c r="F37" s="45"/>
       <c r="G37" s="35"/>
-      <c r="H37" s="37"/>
+      <c r="H37" s="45"/>
       <c r="I37" s="37"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="55"/>
-      <c r="L37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="55"/>
       <c r="M37" s="37"/>
-      <c r="N37" s="19"/>
+      <c r="N37" s="37"/>
       <c r="O37" s="19"/>
-      <c r="P37" s="20"/>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P37" s="19"/>
+      <c r="Q37" s="20"/>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B38" s="18"/>
       <c r="C38" s="19"/>
       <c r="D38" s="44"/>
       <c r="E38" s="44"/>
       <c r="F38" s="45"/>
       <c r="G38" s="35"/>
-      <c r="H38" s="37"/>
+      <c r="H38" s="45"/>
       <c r="I38" s="37"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="55"/>
-      <c r="L38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="55"/>
       <c r="M38" s="37"/>
-      <c r="N38" s="19"/>
+      <c r="N38" s="37"/>
       <c r="O38" s="19"/>
-      <c r="P38" s="20"/>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P38" s="19"/>
+      <c r="Q38" s="20"/>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B39" s="18"/>
       <c r="C39" s="19"/>
       <c r="D39" s="44"/>
       <c r="E39" s="44"/>
       <c r="F39" s="45"/>
       <c r="G39" s="35"/>
-      <c r="H39" s="37"/>
+      <c r="H39" s="45"/>
       <c r="I39" s="37"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="55"/>
-      <c r="L39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="55"/>
       <c r="M39" s="37"/>
-      <c r="N39" s="19"/>
+      <c r="N39" s="37"/>
       <c r="O39" s="19"/>
-      <c r="P39" s="20"/>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P39" s="19"/>
+      <c r="Q39" s="20"/>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B40" s="18"/>
       <c r="C40" s="19"/>
       <c r="D40" s="44"/>
       <c r="E40" s="44"/>
       <c r="F40" s="45"/>
       <c r="G40" s="35"/>
-      <c r="H40" s="37"/>
+      <c r="H40" s="45"/>
       <c r="I40" s="37"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="55"/>
-      <c r="L40" s="37"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="55"/>
       <c r="M40" s="37"/>
-      <c r="N40" s="19"/>
+      <c r="N40" s="37"/>
       <c r="O40" s="19"/>
-      <c r="P40" s="20"/>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P40" s="19"/>
+      <c r="Q40" s="20"/>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B41" s="18"/>
       <c r="C41" s="19"/>
       <c r="D41" s="44"/>
       <c r="E41" s="44"/>
       <c r="F41" s="45"/>
       <c r="G41" s="35"/>
-      <c r="H41" s="37"/>
+      <c r="H41" s="45"/>
       <c r="I41" s="37"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="55"/>
-      <c r="L41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="55"/>
       <c r="M41" s="37"/>
-      <c r="N41" s="19"/>
+      <c r="N41" s="37"/>
       <c r="O41" s="19"/>
-      <c r="P41" s="20"/>
-    </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P41" s="19"/>
+      <c r="Q41" s="20"/>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B42" s="18"/>
       <c r="C42" s="19"/>
       <c r="D42" s="44"/>
       <c r="E42" s="44"/>
       <c r="F42" s="45"/>
       <c r="G42" s="35"/>
-      <c r="H42" s="37"/>
+      <c r="H42" s="45"/>
       <c r="I42" s="37"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="55"/>
-      <c r="L42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="55"/>
       <c r="M42" s="37"/>
-      <c r="N42" s="19"/>
+      <c r="N42" s="37"/>
       <c r="O42" s="19"/>
-      <c r="P42" s="20"/>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P42" s="19"/>
+      <c r="Q42" s="20"/>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B43" s="18"/>
       <c r="C43" s="19"/>
       <c r="D43" s="44"/>
       <c r="E43" s="44"/>
       <c r="F43" s="45"/>
       <c r="G43" s="35"/>
-      <c r="H43" s="37"/>
+      <c r="H43" s="45"/>
       <c r="I43" s="37"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="55"/>
-      <c r="L43" s="37"/>
+      <c r="J43" s="37"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="55"/>
       <c r="M43" s="37"/>
-      <c r="N43" s="19"/>
+      <c r="N43" s="37"/>
       <c r="O43" s="19"/>
-      <c r="P43" s="20"/>
-    </row>
-    <row r="44" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P43" s="19"/>
+      <c r="Q43" s="20"/>
+    </row>
+    <row r="44" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="22"/>
       <c r="C44" s="23"/>
       <c r="D44" s="47"/>
       <c r="E44" s="47"/>
       <c r="F44" s="48"/>
       <c r="G44" s="49"/>
-      <c r="H44" s="50"/>
+      <c r="H44" s="48"/>
       <c r="I44" s="50"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="56"/>
-      <c r="L44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="23"/>
+      <c r="L44" s="56"/>
       <c r="M44" s="50"/>
-      <c r="N44" s="23"/>
+      <c r="N44" s="50"/>
       <c r="O44" s="23"/>
-      <c r="P44" s="24"/>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="J45" s="8"/>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="J46" s="8"/>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="J47" s="8"/>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="J48" s="8"/>
-    </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J49" s="8"/>
-    </row>
-    <row r="50" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J50" s="8"/>
-    </row>
-    <row r="51" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J51" s="8"/>
-    </row>
-    <row r="52" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J52" s="8"/>
+      <c r="P44" s="23"/>
+      <c r="Q44" s="24"/>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="K45" s="8"/>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="K46" s="8"/>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="K47" s="8"/>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="K48" s="8"/>
+    </row>
+    <row r="49" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K49" s="8"/>
+    </row>
+    <row r="50" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K50" s="8"/>
+    </row>
+    <row r="51" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K51" s="8"/>
+    </row>
+    <row r="52" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K52" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3266,7 +3316,7 @@
           <x14:formula1>
             <xm:f>About!$B$3:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J4:J44</xm:sqref>
+          <xm:sqref>K4:K44</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3308,34 +3358,34 @@
         <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -3343,34 +3393,34 @@
         <v>87</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="F3" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="G3" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="K3" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="L3" s="17" t="s">
         <v>120</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -4006,7 +4056,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4024,7 +4074,7 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -4046,13 +4096,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
         <v>110</v>
-      </c>
-      <c r="C4" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>